<commit_message>
Map Date into Excel date number back
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/accountBills.xlsx
+++ b/tests/resources/xlsx/accountBills.xlsx
@@ -5,17 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\skipped-bills\tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\skipped-bills\tests\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA4943C-9F36-4431-96B4-4533B14168AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5105A87C-15BB-4767-8FB5-4BB46F1F65E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -189,47 +189,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D210C99C-A905-4E41-A64D-F1CB2B864A2A}"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -248,10 +208,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,7 +535,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -679,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>44565</v>
+        <v>44566</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>10</v>
@@ -696,10 +652,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$F2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rename account bills' "Date" to "Transfer date"
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/accountBills.xlsx
+++ b/tests/resources/xlsx/accountBills.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\skipped-bills\tests\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8571AF2A-A0CD-4770-B7D9-75218D08AAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C00F0D-4258-4DEF-8C34-1821EB32627A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -80,10 +80,10 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Amount</t>
+  </si>
+  <si>
+    <t>Transfer date</t>
   </si>
 </sst>
 </file>
@@ -174,27 +174,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{D210C99C-A905-4E41-A64D-F1CB2B864A2A}"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -540,7 +520,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -559,13 +539,13 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>13</v>
@@ -645,7 +625,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$E2&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implement account bills rules handler
Now you can write a set of rules to apply on account bills.
The rules handler specify:
- the structure
- collection operators
- element operators
- the output if a rule is matched
</commit_message>
<xml_diff>
--- a/tests/resources/xlsx/accountBills.xlsx
+++ b/tests/resources/xlsx/accountBills.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\skipped-bills\tests\resources\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C00F0D-4258-4DEF-8C34-1821EB32627A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5515B93-EAEF-4056-885E-360D277AFC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="888" windowWidth="13800" windowHeight="7092" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -44,12 +44,6 @@
     <t>account B</t>
   </si>
   <si>
-    <t>Title: 0090729</t>
-  </si>
-  <si>
-    <t>Title: 00091840</t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
@@ -62,9 +56,6 @@
     <t>2022-01-02</t>
   </si>
   <si>
-    <t>Title: 0090744</t>
-  </si>
-  <si>
     <t>Shop</t>
   </si>
   <si>
@@ -84,6 +75,15 @@
   </si>
   <si>
     <t>Transfer date</t>
+  </si>
+  <si>
+    <t>Title: 0090729 in ABC</t>
+  </si>
+  <si>
+    <t>Title: 0090744 in ABC</t>
+  </si>
+  <si>
+    <t>Title: 00091840 in Little Shop</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -528,44 +528,44 @@
     <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="6">
         <v>-20.48</v>
@@ -574,21 +574,21 @@
         <v>0</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="6">
         <v>-29.95</v>
@@ -597,12 +597,12 @@
         <v>0</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
@@ -611,7 +611,7 @@
         <v>44566</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6">
         <v>-71.58</v>
@@ -620,7 +620,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>